<commit_message>
Update Budget Plan (version 1).xlsx
</commit_message>
<xml_diff>
--- a/Budget Plan (version 1).xlsx
+++ b/Budget Plan (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\2018 Fall\Capstone\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24DEB84A-582C-42CE-BC0D-ED83695EABF9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7269B4-B319-46E5-B4B7-A7F99D748A84}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="7485" xr2:uid="{FDC3888E-3DAD-46E2-8782-7814584CFEBB}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Parts</t>
   </si>
@@ -61,26 +60,50 @@
     <t>1,621 RPM HD Premium Planetary Gear Motor</t>
   </si>
   <si>
-    <t>6061-T6511 Aluminum Flat(31/16 X 6X 18)</t>
-  </si>
-  <si>
-    <t>Bearings</t>
-  </si>
-  <si>
-    <t>Hot Rolled A-36 Steel Round 30 in</t>
-  </si>
-  <si>
     <t>Total budget</t>
   </si>
   <si>
     <t>6063-T52 Aluminum Rectangle Tube(2X1X1/8 Wall)</t>
+  </si>
+  <si>
+    <t>Driving Belt</t>
+  </si>
+  <si>
+    <t>Pulley</t>
+  </si>
+  <si>
+    <t>Roller Bearing</t>
+  </si>
+  <si>
+    <t>Bearing</t>
+  </si>
+  <si>
+    <t>Gears</t>
+  </si>
+  <si>
+    <t>5" wheels/hubs</t>
+  </si>
+  <si>
+    <t>1/2" Hot Rolled A-36 Steel Round</t>
+  </si>
+  <si>
+    <t>5/8" Hot Rolled A-36 Steel Round</t>
+  </si>
+  <si>
+    <t>Screws</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+11 GA. (.120 thick)
+Hot Rolled Steel Sheet (2'X4')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
@@ -147,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -163,6 +186,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB0FF1C-31FB-48EF-A27D-81D1CDE1C344}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +532,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
@@ -523,8 +550,8 @@
         <v>79.98</v>
       </c>
       <c r="F2" s="2">
-        <f>SUM(D2:D9)</f>
-        <v>411.85999999999996</v>
+        <f>SUM(D:D)</f>
+        <v>726.3</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
@@ -538,7 +565,7 @@
         <v>13.82</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D9" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D17" si="0">B3*C3</f>
         <v>41.46</v>
       </c>
     </row>
@@ -589,7 +616,7 @@
     </row>
     <row r="7" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -602,39 +629,169 @@
         <v>32.15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>9</v>
+    <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" s="2">
-        <v>61.7</v>
+        <v>77</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>61.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>11</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" s="2">
+        <v>5.14</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>5.14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
         <v>6.6</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>6.6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="7">
         <v>10</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>22</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>20</v>
+      </c>
+      <c r="D18" s="2">
+        <f>B18*C18</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>